<commit_message>
Adding Daily Standings to app
</commit_message>
<xml_diff>
--- a/Misc/Colors.xlsx
+++ b/Misc/Colors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aclark/Box/Alissa Private Folder/Alex/PBE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aclark/Documents/GitHub/PBE/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3C501B4-AEF7-1E4D-BC9C-D2D32795497F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8059D81-CE2D-7645-BE50-23F08174A5F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{4F0B26C8-F47D-B948-8786-62AE6A3D71E6}"/>
+    <workbookView xWindow="4060" yWindow="2860" windowWidth="28040" windowHeight="17040" xr2:uid="{4F0B26C8-F47D-B948-8786-62AE6A3D71E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Team</t>
   </si>
@@ -141,25 +141,28 @@
     <t>#D4D4C8</t>
   </si>
   <si>
+    <t>#F0F0F0</t>
+  </si>
+  <si>
+    <t>#16567B</t>
+  </si>
+  <si>
+    <t>#2C0060</t>
+  </si>
+  <si>
+    <t>#183013</t>
+  </si>
+  <si>
+    <t>#808000</t>
+  </si>
+  <si>
+    <t>#C1C1C1</t>
+  </si>
+  <si>
+    <t>team_id</t>
+  </si>
+  <si>
     <t>#115376</t>
-  </si>
-  <si>
-    <t>#F0F0F0</t>
-  </si>
-  <si>
-    <t>#16567B</t>
-  </si>
-  <si>
-    <t>#2C0060</t>
-  </si>
-  <si>
-    <t>#183013</t>
-  </si>
-  <si>
-    <t>#808000</t>
-  </si>
-  <si>
-    <t>#C1C1C1</t>
   </si>
 </sst>
 </file>
@@ -513,201 +516,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1286500-BEF6-F14D-8494-31B2C1D716F8}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update color pallete uses
</commit_message>
<xml_diff>
--- a/Misc/Colors.xlsx
+++ b/Misc/Colors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aclark/Documents/GitHub/PBE/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8059D81-CE2D-7645-BE50-23F08174A5F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ACA9E9-BC5A-B047-9C9C-74B157094E0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4060" yWindow="2860" windowWidth="28040" windowHeight="17040" xr2:uid="{4F0B26C8-F47D-B948-8786-62AE6A3D71E6}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>#000000</t>
   </si>
   <si>
-    <t>#FCEC00</t>
-  </si>
-  <si>
     <t>#6C0000</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>#115376</t>
+  </si>
+  <si>
+    <t>#D0D02B</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,7 +533,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -607,7 +607,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -624,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -641,13 +641,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -658,13 +658,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -675,10 +675,10 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -692,13 +692,13 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -709,13 +709,13 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -726,7 +726,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
@@ -743,13 +743,13 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>40</v>
-      </c>
-      <c r="E13" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>